<commit_message>
Atualização na modelagem do BD e Backlog
</commit_message>
<xml_diff>
--- a/Documentação/Backlog.xlsx
+++ b/Documentação/Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4d8695ce2d52cc0/Área de Trabalho/Pedro/PI/Sprint2/Sprint02/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\Sprint2\Sprint02\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{90E21A04-405A-430C-8E21-BFBA4E5CA5C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5F2FBFC-6817-4A93-AF4C-317EFC926D5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C3C5E6-666A-4F7B-A4D4-FF16E6188FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2C40FE5B-BD07-468D-8865-71C02FCF0329}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Projeto - Harbor Solutions</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Website</t>
   </si>
   <si>
-    <t>Missão/ Valores/ Visão</t>
-  </si>
-  <si>
     <t>dashboard</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>Planilha de Riscos do Projeto</t>
   </si>
   <si>
-    <t>Pagina quem somos nós</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -116,6 +110,9 @@
   </si>
   <si>
     <t>Pagina de cadastro cliente e  login</t>
+  </si>
+  <si>
+    <t>Pagina quem somos nós(Missão/ Valores/ Visão)</t>
   </si>
 </sst>
 </file>
@@ -292,6 +289,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,9 +308,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -676,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182CB990-1A60-4F22-9F2B-8B8E19E3CED8}">
-  <dimension ref="E2:I27"/>
+  <dimension ref="E2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -694,22 +691,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
@@ -732,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="5:9" x14ac:dyDescent="0.25">
@@ -741,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>5</v>
@@ -756,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>5</v>
@@ -782,10 +779,10 @@
         <v>3</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I9" s="6">
         <v>13</v>
@@ -797,10 +794,10 @@
         <v>4</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="6">
         <v>21</v>
@@ -812,10 +809,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I11" s="6">
         <v>21</v>
@@ -827,10 +824,10 @@
         <v>6</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I12" s="6">
         <v>5</v>
@@ -842,13 +839,13 @@
         <v>7</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="8">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="I13" s="6">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="5:9" x14ac:dyDescent="0.25">
@@ -857,116 +854,116 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14" s="6">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="6"/>
-      <c r="F15" s="6">
-        <v>9</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="6">
-        <v>21</v>
-      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="4">
-        <v>3</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E17" s="6"/>
       <c r="F17" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I17" s="6">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E18" s="6"/>
       <c r="F18" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="6"/>
-      <c r="F19" s="6">
-        <v>12</v>
-      </c>
-      <c r="G19" s="6" t="s">
+      <c r="E19" s="4">
+        <v>4</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" s="6">
-        <v>5</v>
-      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="4">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6">
+        <v>13</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="6">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E21" s="6"/>
       <c r="F21" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="I21" s="6">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E22" s="6"/>
       <c r="F22" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>19</v>
@@ -975,77 +972,62 @@
         <v>5</v>
       </c>
       <c r="I22" s="6">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="6"/>
-      <c r="F23" s="6">
-        <v>15</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="6">
-        <v>13</v>
-      </c>
+      <c r="E23" s="4">
+        <v>5</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="4">
-        <v>5</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8">
+        <v>16</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="6">
+        <v>21</v>
+      </c>
     </row>
     <row r="25" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E25" s="8"/>
       <c r="F25" s="8">
-        <v>16</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I25" s="6">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E26" s="8"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="8">
-        <v>17</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="10"/>
-      <c r="F27" s="8">
-        <v>18</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="17">
+        <v>25</v>
+      </c>
+      <c r="I26" s="11">
         <v>21</v>
       </c>
     </row>

</xml_diff>